<commit_message>
fixed calculation of factor
</commit_message>
<xml_diff>
--- a/docs/project_management/risk_assessment.xlsx
+++ b/docs/project_management/risk_assessment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -74,9 +74,6 @@
     </r>
   </si>
   <si>
-    <t>Create prototypes and integration tests</t>
-  </si>
-  <si>
     <t>Loss of back-ups</t>
   </si>
   <si>
@@ -89,8 +86,11 @@
     <t>Missed Milestones</t>
   </si>
   <si>
+    <t xml:space="preserve">Create prototypes and integration tests, </t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Total
+      <t xml:space="preserve">Risk Factor
 </t>
     </r>
     <r>
@@ -103,6 +103,9 @@
       </rPr>
       <t>Likelihood x Impact</t>
     </r>
+  </si>
+  <si>
+    <t>Allow time near end of project to catch-up</t>
   </si>
 </sst>
 </file>
@@ -479,7 +482,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +546,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E8" si="0">SUM(C3*D3)</f>
+        <f t="shared" ref="E3:E21" si="0">SUM(C3*D3)</f>
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -555,7 +558,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
@@ -574,7 +577,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5">
         <v>4</v>
@@ -586,7 +589,9 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -599,11 +604,11 @@
         <v>2</v>
       </c>
       <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
         <v>2</v>
-      </c>
-      <c r="E6" s="5">
-        <f t="shared" si="0"/>
-        <v>4</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -625,7 +630,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -633,7 +638,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="5">
         <v>2</v>
@@ -646,7 +651,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -661,8 +666,8 @@
         <v>1</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" ref="E3:E21" si="1">SUM(C9*2 + D9)</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F9" s="4"/>
     </row>
@@ -678,8 +683,8 @@
         <v>1</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F10" s="4"/>
     </row>
@@ -695,8 +700,8 @@
         <v>1</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F11" s="4"/>
     </row>
@@ -712,8 +717,8 @@
         <v>1</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F12" s="4"/>
     </row>
@@ -729,8 +734,8 @@
         <v>1</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F13" s="4"/>
     </row>
@@ -746,8 +751,8 @@
         <v>1</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F14" s="4"/>
     </row>
@@ -763,8 +768,8 @@
         <v>1</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F15" s="4"/>
     </row>
@@ -780,8 +785,8 @@
         <v>1</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F16" s="4"/>
     </row>
@@ -797,8 +802,8 @@
         <v>1</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F17" s="4"/>
     </row>
@@ -814,8 +819,8 @@
         <v>1</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F18" s="4"/>
     </row>
@@ -831,8 +836,8 @@
         <v>1</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F19" s="4"/>
     </row>
@@ -848,8 +853,8 @@
         <v>1</v>
       </c>
       <c r="E20" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F20" s="4"/>
     </row>
@@ -865,8 +870,8 @@
         <v>1</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F21" s="4"/>
     </row>

</xml_diff>